<commit_message>
added models and img for data visuals
</commit_message>
<xml_diff>
--- a/Backend/static/data/Truck_Fullness_Prediction.xlsx
+++ b/Backend/static/data/Truck_Fullness_Prediction.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbern\OneDrive\Desktop\FedExML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbern\OneDrive\Desktop\FedExML\Backend\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D49B15AC-FC8A-4A65-8966-C9A75EFDEC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64611A1-6610-41E0-B66C-7FBCDCB42180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7206C078-2B8E-4989-BF3E-7C5EAAAE88CF}"/>
   </bookViews>
@@ -23,7 +23,20 @@
     <sheet name="Sheet7" sheetId="8" state="hidden" r:id="rId8"/>
     <sheet name="Sheet8" sheetId="9" state="hidden" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -9487,6 +9500,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.49913692038495189"/>
+                  <c:y val="0.26902413240011663"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet8!$A$101:$A$200</c:f>
@@ -12915,6 +12978,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.13042714822539284"/>
+                  <c:y val="5.2867454068241469E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet2!$A$11:$A$20</c:f>
@@ -23535,6 +23648,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.9028654297796482E-2"/>
+                  <c:y val="4.9150627004957717E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet3!$A$11:$A$20</c:f>
@@ -24646,6 +24809,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.42068462522882388"/>
+                  <c:y val="0.12218666666666667"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet5!$A$11:$A$20</c:f>
@@ -39038,16 +39251,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>108137</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>169769</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>412937</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>55469</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -39377,16 +39590,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -39629,16 +39842,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -39701,16 +39914,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -40275,11 +40488,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4028D5E4-239C-4DB4-AA8E-5EB18EC34622}">
   <dimension ref="A1:XFD1048575"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -40964,8 +41181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A562150-6FBE-4484-AA30-CA9A4043A4E7}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41502,7 +41719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96825928-2D61-4257-902D-AA561C5E1102}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -41603,7 +41820,7 @@
         <v>5</v>
       </c>
       <c r="F7">
-        <v>0.85714443714880173</v>
+        <v>0.85714443714880195</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -42039,8 +42256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F35913E5-85D6-40A8-B038-B948C442A483}">
   <dimension ref="A1:S131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>